<commit_message>
Minor work on BidAI
</commit_message>
<xml_diff>
--- a/Tarot/Assets/ExternalTools/TestsAIs.xlsx
+++ b/Tarot/Assets/ExternalTools/TestsAIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RynikV\Documents\GitHub\Tarot\Tarot\Assets\ExternalTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC981CEB-0BB1-43CD-BC12-C01D144B58B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A258DD42-1C3D-4F6A-97D3-F45FCA4E0271}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" xr2:uid="{4EC411C9-5971-4A85-A892-A4A18CEE9FDB}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
         <v>4.384615384615385</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -601,7 +601,7 @@
         <v>0.92307692307692313</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -640,7 +640,7 @@
         <v>0.92307692307692313</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -658,7 +658,7 @@
         <v>0.92307692307692313</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -677,7 +677,7 @@
       </c>
       <c r="I8">
         <f>E2-SUM(I2:I7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
       </c>
       <c r="I12">
         <f>(I2*$B$2+I3*$B$1+I4*$B$24+I5*$B$25+I6*$B$26+I7*$B$27+IF(I2&gt;=2,$B$3,0)+I8*$B$28)/$E$2</f>
-        <v>3.75</v>
+        <v>3.8888888888888888</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -716,11 +716,11 @@
       </c>
       <c r="H13">
         <f>_xlfn.IFS($E$1=3,$B$5,$E$1=5,$B$6,$E$1=4,1)*(1+$E$7*$E$8)*H12</f>
-        <v>2.1554487179487176</v>
+        <v>2.5865384615384612</v>
       </c>
       <c r="I13">
         <f>_xlfn.IFS($E$1=3,$B$5,$E$1=5,$B$6,$E$1=4,1)*(1+$E$7*$E$8)*I12</f>
-        <v>4.6875</v>
+        <v>5.833333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>